<commit_message>
add clothing_shoes as oc_name option
</commit_message>
<xml_diff>
--- a/data/processed/coarse_data_relational_table.xlsx
+++ b/data/processed/coarse_data_relational_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CClatterbuck\Documents\Github\CAplastics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CClatterbuck\Documents\Github\CAplastics\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0629ABED-78D8-4FAC-9074-1DE0399269C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892462D8-D870-4D10-B2D9-6ACE212196D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="1545" windowWidth="21600" windowHeight="10470" xr2:uid="{637CFD68-AAB6-43B7-BA28-3814684A916B}"/>
+    <workbookView xWindow="840" yWindow="705" windowWidth="21600" windowHeight="11385" xr2:uid="{637CFD68-AAB6-43B7-BA28-3814684A916B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
   <si>
     <t>Cigarette Butts</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>ccd_coarse_name</t>
+  </si>
+  <si>
+    <t>clothing_shoes</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,6 +1215,9 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
       <c r="B46" t="s">
         <v>85</v>
       </c>

</xml_diff>